<commit_message>
Menu is working great
just a few last things to create
</commit_message>
<xml_diff>
--- a/Doc/VX command set.xlsx
+++ b/Doc/VX command set.xlsx
@@ -15,8 +15,139 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D28" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+not implemented yet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D34" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+not implemented yet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D36" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+not implemented yet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D37" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+not implemented yet</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D38" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+not implemented yet
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="85">
   <si>
     <t>Command</t>
   </si>
@@ -54,84 +185,9 @@
     <t>Sub-module</t>
   </si>
   <si>
-    <t>Enable the (cell) Modem</t>
-  </si>
-  <si>
-    <t>Disable the (cell) Modem</t>
-  </si>
-  <si>
-    <t>SR1</t>
-  </si>
-  <si>
-    <t>SR3</t>
-  </si>
-  <si>
-    <t>SR6</t>
-  </si>
-  <si>
-    <t>SR12</t>
-  </si>
-  <si>
-    <t>SR25</t>
-  </si>
-  <si>
-    <t>SR50</t>
-  </si>
-  <si>
-    <t>SR100</t>
-  </si>
-  <si>
-    <t>SR200</t>
-  </si>
-  <si>
-    <t>SR400</t>
-  </si>
-  <si>
-    <t>SR800</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 1HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 3HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 6HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 12HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 25HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 50HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 100HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 200HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 400HZ</t>
-  </si>
-  <si>
-    <t>Change the sample rate to 800HZ</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>Re-initialize the Accelerometer</t>
-  </si>
-  <si>
-    <t>Re-initialize the CAN (STN)</t>
-  </si>
-  <si>
-    <t>Re-initialize the (Cell) Modem</t>
-  </si>
-  <si>
     <t>P</t>
   </si>
   <si>
@@ -168,9 +224,6 @@
     <t>Enable the 5V power supply</t>
   </si>
   <si>
-    <t>Enable the Host power port (requires VXPE5)</t>
-  </si>
-  <si>
     <t>Disable the 3V power supply</t>
   </si>
   <si>
@@ -189,47 +242,198 @@
     <t>Wakeup timer set for xxxxx seconds from now</t>
   </si>
   <si>
-    <t>Disable the Host power port (delay 30 seconds)</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
-    <t>Device Information</t>
-  </si>
-  <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>Device reset</t>
-  </si>
-  <si>
-    <t>Power state information</t>
-  </si>
-  <si>
     <t>W</t>
   </si>
   <si>
     <t>Wake up event query</t>
   </si>
   <si>
-    <t>Modem state information</t>
-  </si>
-  <si>
     <t>CAN state information</t>
+  </si>
+  <si>
+    <t>V2X Device Information</t>
+  </si>
+  <si>
+    <t>Accelerometer X axis offset (zero)</t>
+  </si>
+  <si>
+    <t>Accelerometer Y axis offset (zero)</t>
+  </si>
+  <si>
+    <t>Accelerometer Z axis offset (zero)</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Restart the Accelerometer</t>
+  </si>
+  <si>
+    <t>Modem device information</t>
+  </si>
+  <si>
+    <t>Accelerometer device information</t>
+  </si>
+  <si>
+    <t>CANbus device information</t>
+  </si>
+  <si>
+    <t>Power state query</t>
+  </si>
+  <si>
+    <t>Whole system status query</t>
+  </si>
+  <si>
+    <t>V2X board reset</t>
+  </si>
+  <si>
+    <t>Disable the Modem</t>
+  </si>
+  <si>
+    <t>Enable the Modem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disable wakeup timers </t>
+  </si>
+  <si>
+    <t>Accelerometer state query</t>
+  </si>
+  <si>
+    <t>Modem state query</t>
+  </si>
+  <si>
+    <t>Restart the CAN</t>
+  </si>
+  <si>
+    <t>Rerestart the Modem</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>Change the sample rate to xxx</t>
+  </si>
+  <si>
+    <t>Get single Accelerometer sample</t>
+  </si>
+  <si>
+    <t>Rxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set G-range </t>
+  </si>
+  <si>
+    <t>2, 4, 8, 16</t>
+  </si>
+  <si>
+    <t>1,3,6,12,25,50,100,200,400,800,1600,3200</t>
+  </si>
+  <si>
+    <t>Acceptable inputs</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>XYZT</t>
+  </si>
+  <si>
+    <t>Number confirmed</t>
+  </si>
+  <si>
+    <t>Description of device used</t>
+  </si>
+  <si>
+    <t>"ACL=x" 1=on 0=off</t>
+  </si>
+  <si>
+    <t>"CAN=x" 1=on 0=off</t>
+  </si>
+  <si>
+    <t>Specifies HW and SW revs</t>
+  </si>
+  <si>
+    <t>"OK"</t>
+  </si>
+  <si>
+    <t>Enable the Host power port</t>
+  </si>
+  <si>
+    <t>Disable the Host power port</t>
+  </si>
+  <si>
+    <t>Disable host with delay</t>
+  </si>
+  <si>
+    <t>x: seconds</t>
+  </si>
+  <si>
+    <t>DDx</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>SIMCARD check</t>
+  </si>
+  <si>
+    <t>"SIMPWR=x, SIMNET=x" 1=on 0=off</t>
+  </si>
+  <si>
+    <t>"SIMCARD=x" 1=in 0=out</t>
+  </si>
+  <si>
+    <t>"3V3=x, 4V1=x, 5V0=x, HOST=x" 1=on 0=off</t>
+  </si>
+  <si>
+    <t>All other query results rolled into one</t>
+  </si>
+  <si>
+    <t>Xxxxx</t>
+  </si>
+  <si>
+    <t>Yxxxx</t>
+  </si>
+  <si>
+    <t>Zxxxx</t>
+  </si>
+  <si>
+    <t>Sxxxx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -554,19 +758,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" customWidth="1"/>
+    <col min="5" max="5" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -576,8 +782,14 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="str">
         <f>"VX"&amp;B2&amp;C2</f>
         <v>VXAD</v>
@@ -591,8 +803,15 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2" t="str">
+        <f>"--"</f>
+        <v>--</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>"VX"&amp;B3&amp;C3</f>
         <v>VXAE</v>
@@ -606,203 +825,299 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E6" si="0">"--"</f>
+        <v>--</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="str">
         <f>"VX"&amp;B4&amp;C4</f>
-        <v>VXAR</v>
+        <v>VXAI</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>--</v>
+      </c>
+      <c r="F4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="str">
         <f>"VX"&amp;B5&amp;C5</f>
-        <v>VXASR1</v>
+        <v>VXAQ</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>--</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="str">
         <f>"VX"&amp;B6&amp;C6</f>
-        <v>VXASR100</v>
+        <v>VXAR</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>--</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="str">
         <f>"VX"&amp;B7&amp;C7</f>
-        <v>VXASR12</v>
+        <v>VXASxxxx</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="str">
         <f>"VX"&amp;B8&amp;C8</f>
-        <v>VXASR200</v>
+        <v>VXAXxxxx</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>81</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="E8" t="str">
+        <f>"-127 to 127"</f>
+        <v>-127 to 127</v>
+      </c>
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="str">
         <f>"VX"&amp;B9&amp;C9</f>
-        <v>VXASR25</v>
+        <v>VXAYxxxx</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" ref="E9:E10" si="1">"-127 to 127"</f>
+        <v>-127 to 127</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="str">
         <f>"VX"&amp;B10&amp;C10</f>
-        <v>VXASR3</v>
+        <v>VXAZxxxx</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>-127 to 127</v>
+      </c>
+      <c r="F10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="str">
-        <f>"VX"&amp;B11&amp;C11</f>
-        <v>VXASR400</v>
+        <f t="shared" ref="A11:A12" si="2">"VX"&amp;B11&amp;C11</f>
+        <v>VXAG</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" ref="E11:E23" si="3">"--"</f>
+        <v>--</v>
+      </c>
+      <c r="F11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="str">
-        <f>"VX"&amp;B12&amp;C12</f>
-        <v>VXASR50</v>
+        <f t="shared" si="2"/>
+        <v>VXARxx</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>19</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="E12" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="str">
         <f>"VX"&amp;B13&amp;C13</f>
-        <v>VXASR6</v>
+        <v>VXCD</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="str">
         <f>"VX"&amp;B14&amp;C14</f>
-        <v>VXASR800</v>
+        <v>VXCE</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="str">
         <f>"VX"&amp;B15&amp;C15</f>
-        <v>VXCD</v>
+        <v>VXCI</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="str">
         <f>"VX"&amp;B16&amp;C16</f>
-        <v>VXCE</v>
+        <v>VXCQ</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="str">
         <f>"VX"&amp;B17&amp;C17</f>
         <v>VXCR</v>
@@ -811,281 +1126,434 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>12</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="str">
         <f>"VX"&amp;B18&amp;C18</f>
-        <v>VXMD</v>
+        <v>VXI</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="str">
         <f>"VX"&amp;B19&amp;C19</f>
-        <v>VXME</v>
+        <v>VXMD</v>
       </c>
       <c r="B19" t="s">
         <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="str">
         <f>"VX"&amp;B20&amp;C20</f>
-        <v>VXMR</v>
+        <v>VXME</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>48</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="str">
         <f>"VX"&amp;B21&amp;C21</f>
-        <v>VXPD3</v>
+        <v>VXMI</v>
       </c>
       <c r="B21" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="str">
         <f>"VX"&amp;B22&amp;C22</f>
-        <v>VXPD4</v>
+        <v>VXMQ</v>
       </c>
       <c r="B22" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D22" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="str">
         <f>"VX"&amp;B23&amp;C23</f>
-        <v>VXPD5</v>
+        <v>VXMR</v>
       </c>
       <c r="B23" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="D23" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E23" t="str">
+        <f t="shared" si="3"/>
+        <v>--</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="str">
         <f>"VX"&amp;B24&amp;C24</f>
-        <v>VXPDH</v>
+        <v>VXPD3</v>
       </c>
       <c r="B24" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="str">
         <f>"VX"&amp;B25&amp;C25</f>
-        <v>VXPE3</v>
+        <v>VXPD4</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="str">
         <f>"VX"&amp;B26&amp;C26</f>
-        <v>VXPE4</v>
+        <v>VXPD5</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="str">
         <f>"VX"&amp;B27&amp;C27</f>
-        <v>VXPE5</v>
+        <v>VXPDH</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D27" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="str">
         <f>"VX"&amp;B28&amp;C28</f>
-        <v>VXPEH</v>
+        <v>VXPDDx</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="D28" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="str">
         <f>"VX"&amp;B29&amp;C29</f>
+        <v>VXPE3</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" t="str">
+        <f>"VX"&amp;B30&amp;C30</f>
+        <v>VXPE4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>23</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" t="str">
+        <f>"VX"&amp;B31&amp;C31</f>
+        <v>VXPE5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>16</v>
+      </c>
+      <c r="D31" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" t="str">
+        <f>"VX"&amp;B32&amp;C32</f>
+        <v>VXPEH</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" t="str">
+        <f>"VX"&amp;B33&amp;C33</f>
+        <v>VXPQ</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" t="str">
+        <f>"VX"&amp;B34&amp;C34</f>
+        <v>VXW</v>
+      </c>
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" t="str">
+        <f>"VX"&amp;B35&amp;C35</f>
+        <v>VXQ</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" t="s">
+        <v>45</v>
+      </c>
+      <c r="F35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" t="str">
+        <f>"VX"&amp;B36&amp;C36</f>
+        <v>VXTD</v>
+      </c>
+      <c r="B36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" t="str">
+        <f>"VX"&amp;B37&amp;C37</f>
         <v>VXTWxxxxx</v>
       </c>
-      <c r="B29" t="s">
-        <v>54</v>
-      </c>
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
-      <c r="D29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <f t="shared" ref="A3:A35" si="0">"VX"&amp;B30&amp;C30</f>
-        <v>VXI</v>
-      </c>
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <f t="shared" si="0"/>
-        <v>VXZ</v>
-      </c>
-      <c r="B31" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <f t="shared" si="0"/>
-        <v>VXPI</v>
-      </c>
-      <c r="B32" t="s">
-        <v>38</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="str">
-        <f t="shared" si="0"/>
-        <v>VXPW</v>
-      </c>
-      <c r="B33" t="s">
-        <v>38</v>
-      </c>
-      <c r="C33" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="str">
-        <f t="shared" si="0"/>
-        <v>VXMI</v>
-      </c>
-      <c r="B34" t="s">
-        <v>10</v>
-      </c>
-      <c r="C34" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="str">
-        <f t="shared" si="0"/>
-        <v>VXCI</v>
-      </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" t="s">
-        <v>58</v>
-      </c>
-      <c r="D35" t="s">
-        <v>66</v>
+      <c r="B37" t="s">
+        <v>28</v>
+      </c>
+      <c r="C37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D37" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" t="str">
+        <f>"VX"&amp;B38&amp;C38</f>
+        <v>VXR</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" t="str">
+        <f t="shared" ref="A39:A41" si="4">"VX"&amp;B39&amp;C39</f>
+        <v>VXS</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>76</v>
+      </c>
+      <c r="F39" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" t="str">
+        <f t="shared" si="4"/>
+        <v>VX</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" t="str">
+        <f t="shared" si="4"/>
+        <v>VX</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:D29">
-    <sortCondition ref="A2:A29"/>
+  <sortState ref="A2:D45">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>